<commit_message>
planilha modificada com mais setores
</commit_message>
<xml_diff>
--- a/assets/ttst_ct.xlsx
+++ b/assets/ttst_ct.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="167">
   <si>
     <t xml:space="preserve">CO</t>
   </si>
@@ -173,6 +173,354 @@
   </si>
   <si>
     <t xml:space="preserve">OBS 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S04P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4-8B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A6-6B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S04R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MDI e FL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A6-6A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA e FL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3-3B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA e MDI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3-1B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S05P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FL e SR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2-3A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CT e SR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3-9A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CT e FL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5-4A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S05R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST e FL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A6-10A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4-5B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CT e ST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A6-4B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S06P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST e SFS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5-9A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC e SFS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2-4B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC e ST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S06R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3-6B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A6-5B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A8-6B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S07P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC e PI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3-1A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CP e PI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4-3A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CP e PC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7-9B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S07R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4-7A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7-10B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A6-3B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S08P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PI e BQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A6-4A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC e BQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2-10B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A6-3A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S08R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC e VG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5-1A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BQ e VG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3-2B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BQ e PC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4-6B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S09P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7-10A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3-9B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S09R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7-1A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2-3B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S10P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2-10A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS e SR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4-2B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS e CT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5-8B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 50</t>
   </si>
 </sst>
 </file>
@@ -184,7 +532,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Nimbus Sans"/>
@@ -205,11 +553,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Nimbus Sans"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -254,7 +597,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -264,10 +607,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -296,13 +635,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L51" activeCellId="0" sqref="L51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.8"/>
@@ -348,7 +687,7 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="2" t="n">
         <v>126.75</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -427,7 +766,7 @@
       <c r="G4" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="4" t="n">
+      <c r="H4" s="3" t="n">
         <v>126.75</v>
       </c>
       <c r="I4" s="0" t="s">
@@ -523,7 +862,7 @@
       <c r="G7" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="5" t="n">
+      <c r="H7" s="4" t="n">
         <v>135.9</v>
       </c>
       <c r="I7" s="0" t="s">
@@ -555,7 +894,7 @@
       <c r="G8" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="5" t="n">
+      <c r="H8" s="4" t="n">
         <v>135.9</v>
       </c>
       <c r="I8" s="0" t="s">
@@ -572,7 +911,7 @@
       <c r="B9" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="4" t="n">
         <v>126.1</v>
       </c>
       <c r="D9" s="0" t="s">
@@ -587,7 +926,7 @@
       <c r="G9" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="5" t="n">
+      <c r="H9" s="4" t="n">
         <v>127.5</v>
       </c>
       <c r="I9" s="0" t="s">
@@ -604,7 +943,7 @@
       <c r="B10" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" s="4" t="n">
         <v>126.1</v>
       </c>
       <c r="D10" s="0" t="s">
@@ -619,7 +958,7 @@
       <c r="G10" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="5" t="n">
+      <c r="H10" s="4" t="n">
         <v>127.5</v>
       </c>
       <c r="I10" s="0" t="s">
@@ -636,7 +975,7 @@
       <c r="B11" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="4" t="n">
         <v>126.1</v>
       </c>
       <c r="D11" s="0" t="s">
@@ -651,7 +990,7 @@
       <c r="G11" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="5" t="n">
+      <c r="H11" s="4" t="n">
         <v>127.5</v>
       </c>
       <c r="I11" s="0" t="s">
@@ -668,7 +1007,7 @@
       <c r="B12" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="5" t="n">
+      <c r="C12" s="4" t="n">
         <v>127.5</v>
       </c>
       <c r="D12" s="0" t="s">
@@ -683,7 +1022,7 @@
       <c r="G12" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="5" t="n">
+      <c r="H12" s="4" t="n">
         <v>126.1</v>
       </c>
       <c r="I12" s="0" t="s">
@@ -700,7 +1039,7 @@
       <c r="B13" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="5" t="n">
+      <c r="C13" s="4" t="n">
         <v>127.5</v>
       </c>
       <c r="D13" s="0" t="s">
@@ -715,7 +1054,7 @@
       <c r="G13" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="4" t="n">
+      <c r="H13" s="3" t="n">
         <v>126.1</v>
       </c>
       <c r="I13" s="0" t="s">
@@ -732,7 +1071,7 @@
       <c r="B14" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="5" t="n">
+      <c r="C14" s="4" t="n">
         <v>127.5</v>
       </c>
       <c r="D14" s="0" t="s">
@@ -747,7 +1086,7 @@
       <c r="G14" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="4" t="n">
+      <c r="H14" s="3" t="n">
         <v>126.1</v>
       </c>
       <c r="I14" s="0" t="s">
@@ -755,6 +1094,1143 @@
       </c>
       <c r="J14" s="0" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4" t="n">
+        <v>128.45</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="4" t="n">
+        <v>128.45</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="4" t="n">
+        <v>135.85</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="4" t="n">
+        <v>135.85</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="4" t="n">
+        <v>128.45</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="4" t="n">
+        <v>135.85</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="4" t="n">
+        <v>128.45</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="4" t="n">
+        <v>135.85</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="4" t="n">
+        <v>125.4</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="3" t="n">
+        <v>124.4</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="4" t="n">
+        <v>125.4</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="3" t="n">
+        <v>124.4</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="4" t="n">
+        <v>125.4</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="4" t="n">
+        <v>124.4</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3" t="n">
+        <v>125.4</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="4" t="n">
+        <v>124.4</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="4" t="n">
+        <v>124.4</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3" t="n">
+        <v>125.4</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="4" t="n">
+        <v>128.4</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="4" t="n">
+        <v>127.05</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="4" t="n">
+        <v>128.4</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="4" t="n">
+        <v>127.05</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="4" t="n">
+        <v>128.4</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="4" t="n">
+        <v>127.05</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29" s="4" t="n">
+        <v>128.4</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="4" t="n">
+        <v>127.05</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H30" s="4" t="n">
+        <v>128.4</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="4" t="n">
+        <v>127.05</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="J31" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="3" t="n">
+        <v>133.4</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="4" t="n">
+        <v>133.6</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="3" t="n">
+        <v>133.4</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" s="4" t="n">
+        <v>133.6</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="3" t="n">
+        <v>133.4</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" s="4" t="n">
+        <v>133.6</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="J34" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" s="4" t="n">
+        <v>133.6</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H35" s="3" t="n">
+        <v>133.4</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="4" t="n">
+        <v>133.6</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H36" s="3" t="n">
+        <v>133.4</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" s="4" t="n">
+        <v>133.6</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H37" s="3" t="n">
+        <v>133.4</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="4" t="n">
+        <v>125.35</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H38" s="4" t="n">
+        <v>124</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" s="4" t="n">
+        <v>125.35</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="C40" s="4" t="n">
+        <v>125.35</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H40" s="4" t="n">
+        <v>124</v>
+      </c>
+      <c r="I40" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="J40" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="C41" s="4" t="n">
+        <v>124</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" s="4" t="n">
+        <v>125.35</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="4" t="n">
+        <v>124</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H42" s="4" t="n">
+        <v>125.35</v>
+      </c>
+      <c r="I42" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C43" s="4" t="n">
+        <v>124</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C44" s="3" t="n">
+        <v>132.8</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="3" t="n">
+        <v>132.8</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H45" s="3" t="n">
+        <v>126.5</v>
+      </c>
+      <c r="I45" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="J45" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" s="3" t="n">
+        <v>126.5</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H46" s="3" t="n">
+        <v>132.8</v>
+      </c>
+      <c r="I46" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="J46" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" s="3" t="n">
+        <v>126.5</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H47" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I47" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="J47" s="0" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C48" s="3" t="n">
+        <v>126.95</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G48" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H48" s="4" t="n">
+        <v>128.25</v>
+      </c>
+      <c r="I48" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="J48" s="0" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C49" s="3" t="n">
+        <v>126.95</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H49" s="4" t="n">
+        <v>128.25</v>
+      </c>
+      <c r="I49" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="J49" s="0" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" s="3" t="n">
+        <v>126.95</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I50" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
planilha com ACC e CMV
</commit_message>
<xml_diff>
--- a/assets/ttst_ct.xlsx
+++ b/assets/ttst_ct.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="365">
   <si>
     <t xml:space="preserve">CO</t>
   </si>
@@ -521,6 +521,600 @@
   </si>
   <si>
     <t xml:space="preserve">Obs 50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S10R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KP e CT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2-4A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A6-2B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS e KP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3-3A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S11P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SR e TL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2-6A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS e TL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7-2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A8-9A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S11R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KP e TN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4-1A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS e TN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5-5A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3-8A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S12P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LO e TL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A6-2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JG e TL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7-5A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JG e LO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3-2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S12R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LO e TN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4-7B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JG e TN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4-8A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A6-5A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S13P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JG e JT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A8-5A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CX e JT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2-9B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CX e JG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7-3B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S13R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A8-5B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7-4A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4-9A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S14P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM e PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A8-6A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CX e PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3-10B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CX e CM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4-10B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S14R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5-7A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JG e PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2-5B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JG e CM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A8-2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S15P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A8-3A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A8-8A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S15R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JG e PP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A8-7A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LO e PP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5-7B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LO e JG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A8-8B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5-6A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A8-4B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4-1B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5-2B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S17P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CT e GP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7-8A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS e GP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2-6B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A8-4A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S17R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2-5A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3-10A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7-3A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A6-1A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4-2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4-9B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7-5B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2-7A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2-8A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4-4A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7-6A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5-8A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3-5B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4-10A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5-2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A8-1A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3-6A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A6-8B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A6-7B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2-1B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2-7B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4-4B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5-10B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7-6B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7-8B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2-8B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4-5A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5-10A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A6-1B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7-4B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7-7B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4-6A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2-9A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs 122</t>
   </si>
 </sst>
 </file>
@@ -635,13 +1229,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J122"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L51" activeCellId="0" sqref="L51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A98" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I122" activeCellId="0" sqref="I122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.8"/>
@@ -2098,6 +2692,9 @@
       <c r="C46" s="3" t="n">
         <v>126.5</v>
       </c>
+      <c r="D46" s="0" t="s">
+        <v>32</v>
+      </c>
       <c r="E46" s="0" t="s">
         <v>152</v>
       </c>
@@ -2127,6 +2724,9 @@
       <c r="C47" s="3" t="n">
         <v>126.5</v>
       </c>
+      <c r="D47" s="0" t="s">
+        <v>7</v>
+      </c>
       <c r="E47" s="0" t="s">
         <v>152</v>
       </c>
@@ -2156,6 +2756,9 @@
       <c r="C48" s="3" t="n">
         <v>126.95</v>
       </c>
+      <c r="D48" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="E48" s="0" t="s">
         <v>158</v>
       </c>
@@ -2185,6 +2788,9 @@
       <c r="C49" s="3" t="n">
         <v>126.95</v>
       </c>
+      <c r="D49" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="E49" s="0" t="s">
         <v>158</v>
       </c>
@@ -2214,6 +2820,9 @@
       <c r="C50" s="3" t="n">
         <v>126.95</v>
       </c>
+      <c r="D50" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="E50" s="0" t="s">
         <v>158</v>
       </c>
@@ -2231,6 +2840,2310 @@
       </c>
       <c r="J50" s="0" t="s">
         <v>166</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C51" s="4" t="n">
+        <v>128.25</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H51" s="3" t="n">
+        <v>126.95</v>
+      </c>
+      <c r="I51" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="J51" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C52" s="4" t="n">
+        <v>128.25</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H52" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I52" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="J52" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53" s="4" t="n">
+        <v>128.25</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H53" s="3" t="n">
+        <v>126.95</v>
+      </c>
+      <c r="I53" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="J53" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C54" s="4" t="n">
+        <v>135.1</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="G54" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <v>125.075</v>
+      </c>
+      <c r="I54" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="J54" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C55" s="4" t="n">
+        <v>135.1</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H55" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I55" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="J55" s="0" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="C56" s="4" t="n">
+        <v>135.1</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="G56" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H56" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I56" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="J56" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>125.075</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="G57" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H57" s="4" t="n">
+        <v>135.1</v>
+      </c>
+      <c r="I57" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="J57" s="0" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>125.075</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="G58" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H58" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I58" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="J58" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>125.075</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="G59" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H59" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I59" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="J59" s="0" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="C60" s="4" t="n">
+        <v>133.5</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="G60" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H60" s="0" t="n">
+        <v>124.275</v>
+      </c>
+      <c r="I60" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="J60" s="0" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="C61" s="4" t="n">
+        <v>133.5</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="G61" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H61" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I61" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="J61" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="C62" s="4" t="n">
+        <v>133.5</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="G62" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H62" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I62" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="J62" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>124.275</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="G63" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H63" s="4" t="n">
+        <v>133.5</v>
+      </c>
+      <c r="I63" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="J63" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>124.275</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="G64" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H64" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I64" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="J64" s="0" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>124.275</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="G65" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H65" s="4" t="n">
+        <v>133.5</v>
+      </c>
+      <c r="I65" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="J65" s="0" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C66" s="3" t="n">
+        <v>129.25</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="G66" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H66" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I66" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="J66" s="0" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="C67" s="3" t="n">
+        <v>129.25</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="G67" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H67" s="3" t="n">
+        <v>123.7</v>
+      </c>
+      <c r="I67" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="J67" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C68" s="3" t="n">
+        <v>129.25</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="G68" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H68" s="3" t="n">
+        <v>123.7</v>
+      </c>
+      <c r="I68" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="J68" s="0" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C69" s="3" t="n">
+        <v>123.7</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H69" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I69" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="J69" s="0" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="C70" s="3" t="n">
+        <v>123.7</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="G70" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H70" s="3" t="n">
+        <v>129.25</v>
+      </c>
+      <c r="I70" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="J70" s="0" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C71" s="3" t="n">
+        <v>123.7</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="G71" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H71" s="3" t="n">
+        <v>129.25</v>
+      </c>
+      <c r="I71" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="J71" s="0" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C72" s="4" t="n">
+        <v>128.15</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="F72" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H72" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I72" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="J72" s="0" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="C73" s="4" t="n">
+        <v>128.15</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="G73" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H73" s="3" t="n">
+        <v>124.85</v>
+      </c>
+      <c r="I73" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="J73" s="0" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="C74" s="4" t="n">
+        <v>128.15</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="F74" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="G74" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H74" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I74" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="J74" s="0" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="C75" s="3" t="n">
+        <v>124.85</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="G75" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H75" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I75" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="J75" s="0" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="C76" s="3" t="n">
+        <v>124.85</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F76" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="G76" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H76" s="4" t="n">
+        <v>128.15</v>
+      </c>
+      <c r="I76" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="J76" s="0" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="C77" s="3" t="n">
+        <v>124.85</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F77" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="G77" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H77" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I77" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="J77" s="0" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="C78" s="4" t="n">
+        <v>128.35</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="G78" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H78" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I78" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="J78" s="0" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C79" s="4" t="n">
+        <v>128.35</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E79" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="G79" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H79" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I79" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="J79" s="0" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="C80" s="3" t="n">
+        <v>135.8</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="G80" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H80" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I80" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="J80" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="C81" s="3" t="n">
+        <v>135.8</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E81" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="F81" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="G81" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H81" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I81" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="J81" s="0" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C82" s="3" t="n">
+        <v>135.8</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="G82" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H82" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I82" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="J82" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="C83" s="4" t="n">
+        <v>124.9</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E83" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="F83" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="G83" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H83" s="4" t="n">
+        <v>133.8</v>
+      </c>
+      <c r="I83" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="J83" s="0" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="C84" s="4" t="n">
+        <v>124.9</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="F84" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="G84" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H84" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I84" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="J84" s="0" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="C85" s="4" t="n">
+        <v>133.8</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="F85" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="G85" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H85" s="4" t="n">
+        <v>124.9</v>
+      </c>
+      <c r="I85" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="J85" s="0" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="C86" s="4" t="n">
+        <v>133.8</v>
+      </c>
+      <c r="D86" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E86" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="F86" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="G86" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H86" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I86" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="J86" s="0" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C87" s="3" t="n">
+        <v>125.8</v>
+      </c>
+      <c r="D87" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E87" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="F87" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="G87" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H87" s="4" t="n">
+        <v>127.2</v>
+      </c>
+      <c r="I87" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="J87" s="0" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C88" s="3" t="n">
+        <v>125.8</v>
+      </c>
+      <c r="D88" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E88" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="F88" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="G88" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H88" s="4" t="n">
+        <v>127.2</v>
+      </c>
+      <c r="I88" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="J88" s="0" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="C89" s="3" t="n">
+        <v>125.8</v>
+      </c>
+      <c r="D89" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E89" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="F89" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="G89" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H89" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I89" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="J89" s="0" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C90" s="4" t="n">
+        <v>127.2</v>
+      </c>
+      <c r="D90" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E90" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="F90" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="G90" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H90" s="3" t="n">
+        <v>125.8</v>
+      </c>
+      <c r="I90" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="J90" s="0" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C91" s="4" t="n">
+        <v>127.2</v>
+      </c>
+      <c r="D91" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E91" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="F91" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="G91" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H91" s="3" t="n">
+        <v>125.8</v>
+      </c>
+      <c r="I91" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="J91" s="0" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="C92" s="4" t="n">
+        <v>127.2</v>
+      </c>
+      <c r="D92" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E92" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="F92" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="G92" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H92" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I92" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="J92" s="0" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C93" s="4" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="D93" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E93" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="F93" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G93" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H93" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I93" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="J93" s="0" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C94" s="4" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="D94" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E94" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="F94" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G94" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H94" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I94" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="J94" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C95" s="4" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="D95" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E95" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="F95" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G95" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H95" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I95" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="J95" s="0" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C96" s="4" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="D96" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E96" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="F96" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G96" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H96" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I96" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="J96" s="0" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C97" s="4" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="D97" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E97" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="F97" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G97" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H97" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I97" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="J97" s="0" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="C98" s="4" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="D98" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E98" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F98" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G98" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H98" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I98" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="J98" s="0" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="C99" s="4" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="D99" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E99" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F99" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G99" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H99" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I99" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="J99" s="0" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="C100" s="4" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="D100" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E100" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F100" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G100" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H100" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I100" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="J100" s="0" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C101" s="4" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="D101" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E101" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F101" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G101" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H101" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I101" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="J101" s="0" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="C102" s="4" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="D102" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E102" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F102" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G102" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H102" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I102" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="J102" s="0" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C103" s="4" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="D103" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E103" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F103" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G103" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H103" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I103" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="J103" s="0" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C104" s="4" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="D104" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E104" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F104" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G104" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H104" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I104" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="J104" s="0" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="C105" s="4" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="D105" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E105" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F105" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G105" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H105" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I105" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="J105" s="0" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C106" s="4" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="D106" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E106" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="F106" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G106" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H106" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I106" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="J106" s="0" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C107" s="4" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="D107" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E107" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="F107" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G107" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H107" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I107" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="J107" s="0" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C108" s="4" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="D108" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E108" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="F108" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G108" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H108" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I108" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="J108" s="0" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="C109" s="4" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="D109" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E109" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="F109" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G109" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H109" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I109" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="J109" s="0" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C110" s="4" t="n">
+        <v>132.05</v>
+      </c>
+      <c r="D110" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E110" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="F110" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G110" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H110" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I110" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="J110" s="0" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C111" s="4" t="n">
+        <v>132.05</v>
+      </c>
+      <c r="D111" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E111" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="F111" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G111" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H111" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I111" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="J111" s="0" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="B112" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C112" s="4" t="n">
+        <v>132.05</v>
+      </c>
+      <c r="D112" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E112" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="F112" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G112" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H112" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I112" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="J112" s="0" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C113" s="4" t="n">
+        <v>132.05</v>
+      </c>
+      <c r="D113" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E113" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="F113" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G113" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H113" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I113" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="J113" s="0" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C114" s="3" t="n">
+        <v>132.45</v>
+      </c>
+      <c r="D114" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E114" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F114" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G114" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H114" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I114" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="J114" s="0" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="C115" s="3" t="n">
+        <v>132.45</v>
+      </c>
+      <c r="D115" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E115" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F115" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G115" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H115" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I115" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="J115" s="0" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C116" s="3" t="n">
+        <v>132.45</v>
+      </c>
+      <c r="D116" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E116" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F116" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G116" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H116" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I116" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="J116" s="0" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="C117" s="3" t="n">
+        <v>132.45</v>
+      </c>
+      <c r="D117" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E117" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F117" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G117" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H117" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I117" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="J117" s="0" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="n">
+        <v>118</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C118" s="3" t="n">
+        <v>132.45</v>
+      </c>
+      <c r="D118" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E118" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F118" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G118" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H118" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I118" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="J118" s="0" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="n">
+        <v>119</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="C119" s="3" t="n">
+        <v>132.45</v>
+      </c>
+      <c r="D119" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E119" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F119" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G119" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H119" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I119" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="J119" s="0" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C120" s="3" t="n">
+        <v>132.45</v>
+      </c>
+      <c r="D120" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E120" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F120" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G120" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H120" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I120" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="J120" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="n">
+        <v>121</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C121" s="3" t="n">
+        <v>132.45</v>
+      </c>
+      <c r="D121" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E121" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F121" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G121" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H121" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I121" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="J121" s="0" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="C122" s="3" t="n">
+        <v>132.45</v>
+      </c>
+      <c r="D122" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E122" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F122" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G122" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H122" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I122" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="J122" s="0" t="s">
+        <v>364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
planilha atualizada, correcao PF TS para Telesat
</commit_message>
<xml_diff>
--- a/assets/ttst_ct.xlsx
+++ b/assets/ttst_ct.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,6 +33,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Este TF1 é de uso entre o APP-Foz de Iguaçu e o APP-Guarani. Uma ponta do ckt nasce em Foz do Iguaçu, vem até Curitiba, via este canal da OI, e segue para a ponta do Paraguai através do bastidor REDDIG aqui da SATEC (porta 0/1/2).</t>
         </r>
@@ -1385,6 +1386,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CCAM – SGAS</t>
     </r>
@@ -1393,6 +1395,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1403,6 +1406,7 @@
         <color rgb="FFFF6600"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DESATIVADO. MIGRADO PAR AO AMHS</t>
     </r>
@@ -1601,6 +1605,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 508 MDM 4 TIM 3-2
 </t>
@@ -1611,6 +1616,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 005 MDM 2 TIM 2-1</t>
     </r>
@@ -1840,6 +1846,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CCAM – ECM C45   &gt;&gt;&gt;   </t>
     </r>
@@ -1850,6 +1857,7 @@
         <color rgb="FF009933"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">VIA ROUTER CCAM</t>
     </r>
@@ -1878,6 +1886,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 203 MDM 3 TIM 3-1
 </t>
@@ -1888,6 +1897,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 561 MDM 4 TIM 3-2</t>
     </r>
@@ -1916,6 +1926,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 203 MDM 3 TIM 1-2
 </t>
@@ -1926,6 +1937,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 561 MDM 2 TIM 2-1</t>
     </r>
@@ -1942,6 +1954,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RADAR TA-10 - </t>
     </r>
@@ -1950,6 +1963,7 @@
         <sz val="6"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">9,6 Kbps Sync</t>
     </r>
@@ -1977,6 +1991,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CCAM – SAGITARIO - </t>
     </r>
@@ -1986,6 +2001,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4,8Kbps Asy</t>
     </r>
@@ -2002,6 +2018,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RADAR STAR 2000 - </t>
     </r>
@@ -2010,6 +2027,7 @@
         <sz val="6"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">9,6KBps Sync</t>
     </r>
@@ -2020,6 +2038,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 525 MDM 5 TIM 5-1
 </t>
@@ -2030,6 +2049,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 415 MDM 3 TIM 1-1</t>
     </r>
@@ -2043,6 +2063,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RADAR STAR 2000 - </t>
     </r>
@@ -2051,6 +2072,7 @@
         <sz val="6"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">19,2KBps Sync</t>
     </r>
@@ -2067,6 +2089,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">LEP SAGITARIO - </t>
     </r>
@@ -2075,6 +2098,7 @@
         <sz val="6"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">64KBps</t>
     </r>
@@ -2085,6 +2109,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 525 MDM 4 TIM 4-2
 </t>
@@ -2095,6 +2120,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 415 MDM 6 TIM 3-2</t>
     </r>
@@ -2120,6 +2146,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 525 MDM 4 TIM 4-1
 </t>
@@ -2130,6 +2157,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 415 MDM 6 TIM 3-1</t>
     </r>
@@ -2269,6 +2297,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 511 MDM 2 TIM 2-1
 </t>
@@ -2279,6 +2308,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 574 MDM 2 TIM 1-1</t>
     </r>
@@ -2350,6 +2380,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 518 MDM 6 TIM 15-3
 </t>
@@ -2360,6 +2391,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 418 MDM 2 TIM 1-3</t>
     </r>
@@ -2418,6 +2450,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 518 MDM 2 TIM 6-2
 </t>
@@ -2428,6 +2461,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 418 MDM 6 TIM 5-2</t>
     </r>
@@ -2450,6 +2484,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DG1(V30-BL59-1,2,3A,4B/V01-447,448,449)DG2(V35-447,448,449/V23-BL04-NV09)CIND_C111_E/1=AE02_C101_E/2</t>
     </r>
@@ -2459,6 +2494,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[D/3]</t>
     </r>
@@ -2467,6 +2503,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(V05-H09-1,2,3)</t>
     </r>
@@ -2483,6 +2520,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 518 MDM 2 TIM 1-1
 </t>
@@ -2493,6 +2531,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 418 MDM 6 TIM 3-1</t>
     </r>
@@ -2509,6 +2548,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">D04 </t>
     </r>
@@ -2518,6 +2558,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(Desativada. Já foi autorizada a sua retirada da SITTI/DG)
 Aguardando agenda – SO Nelson</t>
@@ -2541,6 +2582,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 518 MDM 2 TIM 1-2
 </t>
@@ -2551,6 +2593,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 418 MDM 6 TIM 4-1</t>
     </r>
@@ -2579,6 +2622,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 518 MDM 6 TIM 12-1
 </t>
@@ -2589,6 +2633,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 418 MDM 2 TIM 1-2</t>
     </r>
@@ -2620,6 +2665,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 518 MDM 6 TIM 13-1
 </t>
@@ -2630,6 +2676,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 418 MDM 2 TIM 6-1</t>
     </r>
@@ -2649,6 +2696,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 518 MDM 2 TIM 6-1
 </t>
@@ -2659,6 +2707,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 418 MDM 6 TIM 4-2</t>
     </r>
@@ -2970,6 +3019,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 518 MDM 4 TIM 14-1
 </t>
@@ -2980,6 +3030,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 421 MDM 2 TIM 1-1</t>
     </r>
@@ -3059,6 +3110,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 516 MDM 7 TIM 5-2
 </t>
@@ -3069,6 +3121,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 421 MDM 6 TIM 1-2</t>
     </r>
@@ -3100,6 +3153,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 518 MDM 3 TIM 3-2
 </t>
@@ -3110,6 +3164,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 421 MDM 4 TIM 3-2</t>
     </r>
@@ -3189,6 +3244,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT518 MDM 5 TIM 4-1
 </t>
@@ -3199,6 +3255,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 421 MDM 3 TIM 5-1</t>
     </r>
@@ -3224,6 +3281,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT518 MDM 3 TIM 2-2
 </t>
@@ -3234,6 +3292,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 421 MDM 4 TIM 2-2</t>
     </r>
@@ -3266,6 +3325,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CCAM (RIOSUL)   &gt;&gt;&gt;   </t>
     </r>
@@ -3276,6 +3336,7 @@
         <color rgb="FF009933"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">VIA ROUTER CCAM</t>
     </r>
@@ -3314,6 +3375,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 420 MDM 5 TIM 5-3
 </t>
@@ -3324,6 +3386,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 428 MDM 4 TIM 5-3</t>
     </r>
@@ -3453,6 +3516,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">119.50 MHz </t>
     </r>
@@ -3462,6 +3526,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(R-AFIS Corumbá - VHF EACEA-MUM)</t>
     </r>
@@ -3481,6 +3546,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">121.50 MHz </t>
     </r>
@@ -3490,6 +3556,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(R-AFIS Corumbá futura) VHF EACEA-MUM</t>
     </r>
@@ -3501,6 +3568,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NC SITTI </t>
     </r>
@@ -3509,6 +3577,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(TCS10597879)</t>
     </r>
@@ -3529,6 +3598,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NC SITTI </t>
     </r>
@@ -3537,6 +3607,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(TCS10597873)</t>
     </r>
@@ -3554,6 +3625,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NC SITTI </t>
     </r>
@@ -3562,6 +3634,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(TCS10597890)</t>
     </r>
@@ -3600,6 +3673,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NC SITTI </t>
     </r>
@@ -3608,6 +3682,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(TCS10597891)</t>
     </r>
@@ -3625,6 +3700,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NC SITTI </t>
     </r>
@@ -3633,6 +3709,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(TCS10597882)</t>
     </r>
@@ -3643,6 +3720,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DG1(V30-BL25-1,2,3A,4B/</t>
     </r>
@@ -3652,6 +3730,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Vxx-Blxx-x,x,xA,xB)DG2(Vxx-Blxx-x,x,xA,xB</t>
     </r>
@@ -3660,6 +3739,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/V24-BL07-NV16)CIND_C105_F/4=UTCM_C100_E/4(V02-H03-4,5,6)</t>
     </r>
@@ -3676,6 +3756,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 519 MDM 2 TIM 1-1
 </t>
@@ -3686,6 +3767,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 412 MDM 3 TIM 5-1</t>
     </r>
@@ -3738,6 +3820,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 519 MDM 2 TIM 2-1
 </t>
@@ -3748,6 +3831,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 412 MDM 3 TIM 6-1</t>
     </r>
@@ -3791,6 +3875,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">119.50 MHz </t>
     </r>
@@ -3800,6 +3885,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(R-AFIS Corumbá - VHF DTCEA-CR)</t>
     </r>
@@ -3819,6 +3905,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">119.50 MHz </t>
     </r>
@@ -3828,6 +3915,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(R-AFIS Corumbá - VHF EACEA-MUM)</t>
     </r>
@@ -3838,6 +3926,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 519 MDM 2 TIM 1-2
 </t>
@@ -3848,6 +3937,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 412 MDM 3 TIM 5-2</t>
     </r>
@@ -3861,6 +3951,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">119.50 MHz </t>
     </r>
@@ -3870,6 +3961,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(R-AFIS Corumbá - VHF DTCEA-CR)</t>
     </r>
@@ -3880,6 +3972,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 519 MDM 2 TIM 2-2
 </t>
@@ -3890,6 +3983,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 412 MDM 3 TIM 6-2</t>
     </r>
@@ -3906,6 +4000,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 519 MDM 7 TIM 7-1
 </t>
@@ -3916,6 +4011,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 412 MDM 5 TIM 10-1</t>
     </r>
@@ -3926,6 +4022,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DG1(V11-29[</t>
     </r>
@@ -3935,6 +4032,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RX</t>
     </r>
@@ -3943,6 +4041,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">],30[</t>
     </r>
@@ -3952,6 +4051,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">TX</t>
     </r>
@@ -3960,6 +4060,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">]/V01-517[</t>
     </r>
@@ -3969,6 +4070,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RX</t>
     </r>
@@ -3977,6 +4079,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">],518[</t>
     </r>
@@ -3986,6 +4089,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">TX</t>
     </r>
@@ -3994,6 +4098,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">])DG2(V35-517[</t>
     </r>
@@ -4003,6 +4108,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RX</t>
     </r>
@@ -4011,6 +4117,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">],518[</t>
     </r>
@@ -4020,6 +4127,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">TX</t>
     </r>
@@ -4028,6 +4136,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">]/V18-BL01-NV13-01[</t>
     </r>
@@ -4037,6 +4146,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">TX</t>
     </r>
@@ -4045,6 +4155,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">],02[</t>
     </r>
@@ -4054,6 +4165,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RX</t>
     </r>
@@ -4062,6 +4174,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">])</t>
     </r>
@@ -4225,6 +4338,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RADAR TA-10 - 9,6</t>
     </r>
@@ -4233,6 +4347,7 @@
         <sz val="7"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">KPS Sync</t>
     </r>
@@ -4243,6 +4358,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 420 MDM 6 TIM 4-3
 </t>
@@ -4253,6 +4369,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 426 MDM 8 TIM 5-3</t>
     </r>
@@ -4266,6 +4383,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RADAR TA-10 - </t>
     </r>
@@ -4274,6 +4392,7 @@
         <sz val="7"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">19,2KBps Sync</t>
     </r>
@@ -4440,6 +4559,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">118.90 MHz </t>
     </r>
@@ -4449,6 +4569,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(SPLIT da FREQ. da TWR-BI p/ o DTCEA-CT)</t>
     </r>
@@ -4510,6 +4631,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">VAGO </t>
     </r>
@@ -4519,6 +4641,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(antes, era D142 SPLIT COL)</t>
     </r>
@@ -4784,6 +4907,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DG2(V32-BL20-10//V35-BL31-10)DG1(V01-BL31-10/V14-BL06-5)SLOT </t>
     </r>
@@ -4793,6 +4917,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">?</t>
     </r>
@@ -4801,6 +4926,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> PORTA </t>
     </r>
@@ -4810,6 +4936,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">??</t>
     </r>
@@ -4818,6 +4945,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">=SLOT </t>
     </r>
@@ -4827,6 +4955,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">?</t>
     </r>
@@ -4835,6 +4964,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> PORTA </t>
     </r>
@@ -4844,6 +4974,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">??</t>
     </r>
@@ -4852,6 +4983,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> (CT)</t>
     </r>
@@ -4956,6 +5088,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 514 MDM 2 TIM 4-1
 </t>
@@ -4966,6 +5099,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 428 MDM 5 TIM 2-2</t>
     </r>
@@ -5069,6 +5203,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 514 MDM 2 TIM 2-1
 </t>
@@ -5079,6 +5214,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 428 MDM 5 TIM 3-1</t>
     </r>
@@ -5116,6 +5252,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 514 MDM 3 TIM 1-1
 </t>
@@ -5126,6 +5263,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 428 MDM 4 TIM 1-2</t>
     </r>
@@ -5157,6 +5295,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DADOS RADAR </t>
     </r>
@@ -5166,6 +5305,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(link direto com o CT, não passa por aqui)</t>
     </r>
@@ -5212,6 +5352,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">135.85 MHz</t>
     </r>
@@ -5221,6 +5362,7 @@
         <color rgb="FFFF6600"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -5231,6 +5373,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 514 MDM 6 TIM 6-1
 </t>
@@ -5241,6 +5384,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 428 MDM 6 TIM 6-1</t>
     </r>
@@ -5270,6 +5414,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 514 MDM 2 TIM 4-2
 </t>
@@ -5280,6 +5425,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 428 MDM 5 TIM 7-1</t>
     </r>
@@ -5323,6 +5469,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 516 MDM 3 TIM 4-2
 </t>
@@ -5333,6 +5480,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 434 MDM 2 TIM 2-1</t>
     </r>
@@ -5436,6 +5584,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT516 MDM 8 TIM 2-1
 </t>
@@ -5446,6 +5595,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 434 MDM 4 TIM 3-1</t>
     </r>
@@ -5462,6 +5612,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 516 MDM 8 TIM 1-2
 </t>
@@ -5472,6 +5623,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 434 MDM 4 TIM 1-2</t>
     </r>
@@ -5491,6 +5643,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 516 MDM 6 TIM 3-1
 </t>
@@ -5501,6 +5654,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 434 MDM 11 TIM 18-1</t>
     </r>
@@ -5514,6 +5668,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">TF-1 APP GUARANI </t>
     </r>
@@ -5524,6 +5679,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(PARAR O MOUDE EM CIMA PARA VER OBSERVAÇÃO)</t>
     </r>
@@ -5543,6 +5699,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 516 MDM 4 TIM 2-2
 </t>
@@ -5553,6 +5710,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 434 MDM 5 TIM 2-2</t>
     </r>
@@ -5569,6 +5727,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 516 MDM 2 TIM 1-1
 </t>
@@ -5579,6 +5738,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 434 MDM 7 TIM 3-2</t>
     </r>
@@ -5592,6 +5752,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 516 MDM 6 TIM 3-2
 </t>
@@ -5602,6 +5763,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 434 MDM 11 TIM 18-2</t>
     </r>
@@ -5706,6 +5868,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">G26 </t>
     </r>
@@ -5714,6 +5877,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Z2</t>
     </r>
@@ -5740,6 +5904,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">G24 </t>
     </r>
@@ -5748,6 +5913,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Z1</t>
     </r>
@@ -5774,6 +5940,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">G27 </t>
     </r>
@@ -5782,6 +5949,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Z3</t>
     </r>
@@ -5799,6 +5967,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">G28 </t>
     </r>
@@ -5807,6 +5976,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Z4</t>
     </r>
@@ -5824,6 +5994,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">G114 </t>
     </r>
@@ -5832,6 +6003,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Z6</t>
     </r>
@@ -5849,6 +6021,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">G29 </t>
     </r>
@@ -5857,6 +6030,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Z5</t>
     </r>
@@ -6095,6 +6269,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 519 MDM 3 TIM 5-1
 </t>
@@ -6105,6 +6280,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 437 MDM 2 TIM 1-1</t>
     </r>
@@ -6226,6 +6402,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 519 MDM 5 TIM 4-2
 </t>
@@ -6236,6 +6413,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 437 MDM 6 TIM 4-2</t>
     </r>
@@ -6300,6 +6478,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 520 MDM 6 TIM 5-1
 </t>
@@ -6310,6 +6489,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 437 MDM 5 TIM 6-1</t>
     </r>
@@ -6326,6 +6506,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT519 MDM 5 TIM 3-1
 </t>
@@ -6336,6 +6517,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 437 MDM 6 TIM 3-1</t>
     </r>
@@ -6364,6 +6546,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 519 MDM 5 TIM 3-2
 </t>
@@ -6374,6 +6557,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 437 MDM 6 TIM 3-2</t>
     </r>
@@ -6393,6 +6577,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 519 MDM 3 TIM 4-1
 </t>
@@ -6403,6 +6588,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 437 MDM 2 TIM 5-1</t>
     </r>
@@ -6419,6 +6605,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 519 MDM 3 TIM 5-2
 </t>
@@ -6429,6 +6616,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 437 MDM 2 TIM 1-2</t>
     </r>
@@ -6448,6 +6636,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 519 MDM 4 TIM 6-1
 </t>
@@ -6458,6 +6647,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 437 MDM 3 TIM 5-2</t>
     </r>
@@ -6477,6 +6667,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 519 MDM 4 TIM 6-2
 </t>
@@ -6487,6 +6678,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 437 MDM 3 TIM 4-1</t>
     </r>
@@ -6506,6 +6698,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 513 MDM 2 TIM 1-1
 </t>
@@ -6516,6 +6709,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 437 MDM4 TIM 6-2</t>
     </r>
@@ -6550,6 +6744,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 201 MDM 2 TIM 5-1
 </t>
@@ -6560,6 +6755,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 718 MDM 4 TIM 3-1</t>
     </r>
@@ -6762,6 +6958,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">D180 </t>
     </r>
@@ -6771,6 +6968,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(antiga 125.80 MHz)</t>
     </r>
@@ -6817,6 +7015,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DG1(V30-BL23-6,7,8A,9B/</t>
     </r>
@@ -6826,6 +7025,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">V35-467,468,469)DG2(V35-467,468,469/</t>
     </r>
@@ -6834,6 +7034,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">V24-BL04-NV02)CIND_C102_F/2=AER5_C100_F/2(V01-H12-7,8,9)</t>
     </r>
@@ -6853,6 +7054,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DG1(V30-BL25-6,7,8A,9B/V35-471,472,473)DG2(V35-</t>
     </r>
@@ -6862,6 +7064,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">471,472,473/</t>
     </r>
@@ -6870,6 +7073,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">V24-BL04-NV08)CIND_C102_G/4=AER5_C100_G/3(V01-H14-4,5,6)</t>
     </r>
@@ -6964,6 +7168,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">APP-LO </t>
     </r>
@@ -6973,6 +7178,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(CONTRATO DE RESPONSABILIDADE DA INFRAERO)</t>
     </r>
@@ -7010,6 +7216,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">APP-ME </t>
     </r>
@@ -7019,6 +7226,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(CONTRATO DE RESPONSABILIDADE DA INFRAERO)</t>
     </r>
@@ -7060,6 +7268,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 507 MDM 6 TIM 4-3
 </t>
@@ -7071,6 +7280,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 301 MDM 2 TIM 1-3</t>
     </r>
@@ -7099,6 +7309,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 507 MDM 8 TIM 5-2
 </t>
@@ -7109,6 +7320,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 301 MDM 8 TIM 6-1</t>
     </r>
@@ -7137,6 +7349,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">COPM 4 OIV </t>
     </r>
@@ -7146,6 +7359,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(Desativado em MN e verificar FRM 2774).</t>
     </r>
@@ -7156,6 +7370,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 507 MDM 5 TIM 3-1
 </t>
@@ -7166,6 +7381,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 301 MDM 16 TIM 24-1</t>
     </r>
@@ -7197,6 +7413,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 507 MDM 5 TIM 2-3
 </t>
@@ -7207,6 +7424,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 301 MDM 16 TIM 21-3</t>
     </r>
@@ -7223,6 +7441,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 420 MDM 3 TIM 3-3
 </t>
@@ -7233,6 +7452,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 405 MDM 5 TIM 2-3</t>
     </r>
@@ -7255,6 +7475,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CCAM TWR -</t>
     </r>
@@ -7263,6 +7484,7 @@
         <sz val="6"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> 2,4KBps Asy</t>
     </r>
@@ -7283,6 +7505,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CCAM AIS - </t>
     </r>
@@ -7291,6 +7514,7 @@
         <sz val="6"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2,4KBps Asy</t>
     </r>
@@ -7358,6 +7582,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 512 MDM 7 TIM 3-2
 </t>
@@ -7368,6 +7593,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 931 MDM 6 TIM 4-1</t>
     </r>
@@ -7381,6 +7607,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 511 MDM 5 TIM 4-3
 </t>
@@ -7391,6 +7618,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 931 MDM 2 TIM 1-3</t>
     </r>
@@ -7431,6 +7659,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 512 MDM 8 TIM 4-3
 </t>
@@ -7441,6 +7670,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 931 MDM 7 TIM 5-3</t>
     </r>
@@ -7497,6 +7727,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">D136 (UHF Sintonizável) </t>
     </r>
@@ -7506,6 +7737,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(antiga D134)</t>
     </r>
@@ -7525,6 +7757,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">D154 </t>
     </r>
@@ -7534,6 +7767,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(antiga D160)</t>
     </r>
@@ -7553,6 +7787,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">D181 </t>
     </r>
@@ -7562,6 +7797,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(antiga D194)</t>
     </r>
@@ -7634,6 +7870,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 517 MDM 4 TIM 3-1
 </t>
@@ -7644,6 +7881,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 451 MDM 2 TIM 1-1</t>
     </r>
@@ -7710,6 +7948,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">124,775 MHz </t>
     </r>
@@ -7719,6 +7958,7 @@
         <color rgb="FFFFFF66"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(FREQ NOVA)</t>
     </r>
@@ -7732,6 +7972,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DG1(V25-BL49-1,2,3A,4A/</t>
     </r>
@@ -7741,6 +7982,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">xxxxxxxxxx</t>
     </r>
@@ -7749,6 +7991,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)DG2(</t>
     </r>
@@ -7758,6 +8001,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">xxxxxxxxx/</t>
     </r>
@@ -7766,6 +8010,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">V24-BL06-NV24)CIND_C105_E/2=AE06_C101_E/2(V03-H23-1,2,3) </t>
     </r>
@@ -7779,6 +8024,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">135,000 MHz </t>
     </r>
@@ -7788,6 +8034,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(FREQ NOVA)</t>
     </r>
@@ -7829,6 +8076,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 524 MDM 8 TIM 4-3
 </t>
@@ -7839,6 +8087,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 441 MDM 7 TIM 2-3</t>
     </r>
@@ -7873,6 +8122,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 524 MDM 7 TIM 2-2
 </t>
@@ -7883,6 +8133,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 441 MDM 3 TIM 7-1</t>
     </r>
@@ -7899,6 +8150,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 524 MDM 7 TIM 1-2
 </t>
@@ -7909,6 +8161,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 441 MDM 3 TIM 2-1</t>
     </r>
@@ -7955,6 +8208,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 524 MDM 7 TIM 1-1
 </t>
@@ -7965,6 +8219,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 441 MDM 3 TIM 1-2</t>
     </r>
@@ -7987,6 +8242,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RLT [CV] A3-02</t>
     </r>
@@ -7996,6 +8252,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">B</t>
     </r>
@@ -8009,6 +8266,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 524 MDM 7 TIM 2-1
 </t>
@@ -8019,6 +8277,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 441 MDM 3 TIM 4-2</t>
     </r>
@@ -8050,6 +8309,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 524 MDM 8 TIM 4-1
 </t>
@@ -8060,6 +8320,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 441 MDM 7 TIM 1-1</t>
     </r>
@@ -8091,6 +8352,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 524 MDM 8 TIM 3-1
 </t>
@@ -8101,6 +8363,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 441 MDM 7 TIM 3-1</t>
     </r>
@@ -8196,6 +8459,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 203 MDM 4 TIM 3-2
 </t>
@@ -8206,6 +8470,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 448 MDM 4 TIM 3-1</t>
     </r>
@@ -8280,6 +8545,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NC SITTI</t>
     </r>
@@ -8288,6 +8554,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> (TCS10597483)</t>
     </r>
@@ -8302,6 +8569,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NC SITTI </t>
     </r>
@@ -8310,6 +8578,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(TCS10597492)</t>
     </r>
@@ -8327,6 +8596,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NC SITTI </t>
     </r>
@@ -8335,6 +8605,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(TCS10597501)</t>
     </r>
@@ -8349,6 +8620,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NC SITTI</t>
     </r>
@@ -8357,6 +8629,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> (TCS10597495)</t>
     </r>
@@ -8380,6 +8653,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NC SITTI </t>
     </r>
@@ -8388,6 +8662,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(TCS10597509)</t>
     </r>
@@ -8414,6 +8689,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NC SITTI </t>
     </r>
@@ -8422,6 +8698,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(TCS10597499)</t>
     </r>
@@ -8454,6 +8731,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NC SITTI</t>
     </r>
@@ -8462,6 +8740,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> (TCS10597494)</t>
     </r>
@@ -8479,6 +8758,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NC SITTI </t>
     </r>
@@ -8487,6 +8767,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(TCS10599410)</t>
     </r>
@@ -8514,6 +8795,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 520 MDM 2 TIM 5-2
 </t>
@@ -8524,6 +8806,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 459 MDM 4 TIM 6-2</t>
     </r>
@@ -8625,6 +8908,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 520 MDM 4 TIM 6-1
 </t>
@@ -8635,6 +8919,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 459 MDM 3 TIM 2-1</t>
     </r>
@@ -8666,6 +8951,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 520 MDM 4 TIM 3-1
 </t>
@@ -8676,6 +8962,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 459 MDM 3 TIM 1-1</t>
     </r>
@@ -8701,6 +8988,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 520 MDM 4 TIM 3-2
 </t>
@@ -8711,6 +8999,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 459 MDM 3 TIM 1-2</t>
     </r>
@@ -8775,6 +9064,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 520 MDM 2 TIM 1-1
 </t>
@@ -8785,6 +9075,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 459 MDM 4 TIM 5-1</t>
     </r>
@@ -8839,6 +9130,7 @@
         <color rgb="FF990000"/>
         <rFont val="Comic Sans MS"/>
         <family val="4"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Serviços desta localidade vêm, atualmente, via Manaus. </t>
     </r>
@@ -8850,6 +9142,7 @@
         <color rgb="FF990000"/>
         <rFont val="Comic Sans MS"/>
         <family val="4"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Vide a localidade de Manaus.</t>
     </r>
@@ -8918,6 +9211,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NC SITTI </t>
     </r>
@@ -8927,6 +9221,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">TCS10597792</t>
     </r>
@@ -8944,6 +9239,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NC SITTI </t>
     </r>
@@ -8953,6 +9249,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">TCS10597790</t>
     </r>
@@ -8970,6 +9267,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NC SITTI</t>
     </r>
@@ -8979,6 +9277,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> TCS10597793</t>
     </r>
@@ -8996,6 +9295,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NC SITTI</t>
     </r>
@@ -9005,6 +9305,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> TCS10597795</t>
     </r>
@@ -9022,6 +9323,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NC SITTI </t>
     </r>
@@ -9031,6 +9333,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">TCS10599411 </t>
     </r>
@@ -9048,6 +9351,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">TIOP(RÉGUA</t>
     </r>
@@ -9056,6 +9360,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">11</t>
     </r>
@@ -9065,6 +9370,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-PORT.</t>
     </r>
@@ -9073,6 +9379,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">03</t>
     </r>
@@ -9082,6 +9389,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)CIND_C120_B/1=UTPM_C100_C/1</t>
     </r>
@@ -9096,6 +9404,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">TIOP(RÉGUA</t>
     </r>
@@ -9104,6 +9413,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">11-PORT.04</t>
     </r>
@@ -9113,6 +9423,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)CIND_C120_B/2=UTPM_C100_C/2</t>
     </r>
@@ -9189,6 +9500,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 521 MDM 6 TIM 12-1
 </t>
@@ -9199,6 +9511,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 554 MDM 6 TIM 6-1</t>
     </r>
@@ -9275,6 +9588,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 521 MDM 7 TIM 14-3
 </t>
@@ -9285,6 +9599,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 554 MDM 5 TIM 11-3</t>
     </r>
@@ -9298,6 +9613,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">STPV – RECIFE( LEP)</t>
     </r>
@@ -9306,6 +9622,7 @@
         <sz val="5"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">- 9,6KBps SYN</t>
     </r>
@@ -9316,6 +9633,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 522 MDM 6 TIM 13-3
 </t>
@@ -9326,6 +9644,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 554 MDM 6 TIM 6-3</t>
     </r>
@@ -9339,6 +9658,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">STPV - ATLANTICO </t>
     </r>
@@ -9347,6 +9667,7 @@
         <sz val="5"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">- 9,6KBps SYN</t>
     </r>
@@ -9357,6 +9678,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 522 MDM 6 TIM 14-3
 </t>
@@ -9367,6 +9689,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 554 MDM 6 TIM 7-3</t>
     </r>
@@ -9383,6 +9706,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 522 MDM 6 TIM 2-3
 </t>
@@ -9393,6 +9717,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 554 MDM 6 TIM 11-3</t>
     </r>
@@ -9589,6 +9914,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 503 MDM 2 TIM 3-2
 </t>
@@ -9599,6 +9925,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 445 MDM 4 TIM 3-1</t>
     </r>
@@ -9618,6 +9945,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 503 MDM 2 TIM 2-1
 </t>
@@ -9628,6 +9956,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 445 MDM 4 TIM 5-1</t>
     </r>
@@ -9647,6 +9976,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 503 MDM 2 TIM 1-1
 </t>
@@ -9657,6 +9987,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 445 MDM 4 TIM 1-1</t>
     </r>
@@ -9704,6 +10035,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 503 MDM 3 TIM 2-2
 </t>
@@ -9714,6 +10046,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 446 MDM 2 TIM 1-1</t>
     </r>
@@ -9760,6 +10093,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 515 MDM 5 TIM 2-2
 </t>
@@ -9770,6 +10104,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 415 MDM 10 TIM 17-2</t>
     </r>
@@ -9786,6 +10121,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 516 MDM 3 TIM 4-1
 </t>
@@ -9796,6 +10132,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 434 MDM 2 TIM 1-1</t>
     </r>
@@ -9810,6 +10147,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Repasse do RADAR LP23M do MDI para FL - 9,6Kbps Sync </t>
     </r>
@@ -9818,6 +10156,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -9828,6 +10167,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(DESATIVADO)</t>
     </r>
@@ -9848,6 +10188,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 520 MDM 3 TIM 2-3
 </t>
@@ -9858,6 +10199,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 459 MDM 4 TIM 5-1</t>
     </r>
@@ -9874,6 +10216,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 518 MDM 8 TIM 14-3
 </t>
@@ -9884,6 +10227,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 472 MDM 5 TIM 10-3</t>
     </r>
@@ -9900,6 +10244,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 516 MDM 5 TIM 5-3
 </t>
@@ -9910,6 +10255,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 472 MDM 5 TIM 6-3</t>
     </r>
@@ -9939,6 +10285,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 525 MDM 7 TIM 6-3
 </t>
@@ -9949,6 +10296,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 415 MDM 8 TIM 5-3</t>
     </r>
@@ -10004,6 +10352,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 517 MDM 5 TIM 4-3
 </t>
@@ -10014,6 +10363,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 472 MDM 7 TIM 2-3</t>
     </r>
@@ -10030,6 +10380,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 518 MDM 8 TIM 13-3
 </t>
@@ -10040,6 +10391,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 472 MDM 5 TIM 7-3</t>
     </r>
@@ -10056,6 +10408,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 520 MDM 7 TIM 6-3
 </t>
@@ -10066,6 +10419,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 459 MDM 7 TIM 3-3</t>
     </r>
@@ -10089,6 +10443,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 514 MDM 3 TIM </t>
     </r>
@@ -10098,6 +10453,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1</t>
     </r>
@@ -10106,6 +10462,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-3
 RTT 428 MDM 4 TIM 2-3</t>
@@ -10175,6 +10532,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 518 MDM 7 TIM 7-2
 </t>
@@ -10185,6 +10543,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 472 MDM 2 TIM 1-2</t>
     </r>
@@ -10213,6 +10572,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 518 MDM 7 TIM7-1
 </t>
@@ -10223,6 +10583,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 472 MDM 2 TIM 1-1</t>
     </r>
@@ -10242,6 +10603,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 518 MDM 7 TIM 3-1
 </t>
@@ -10252,6 +10614,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 472 MDM 2 TIM 3-1</t>
     </r>
@@ -10355,6 +10718,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 518 MDM 7 TIM 11-2
 </t>
@@ -10365,6 +10729,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 472 MDM 2 TIM 2-2</t>
     </r>
@@ -10424,6 +10789,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 522 MDM 4 TIM 11-1
 </t>
@@ -10434,6 +10800,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 442 MDM 2 TIM 1-1</t>
     </r>
@@ -10459,6 +10826,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 522 MDM 4 TIM 11-2
 </t>
@@ -10469,6 +10837,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 150 MDM 9 TIM 10-1</t>
     </r>
@@ -10539,6 +10908,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 521 MDM 5 TIM 5-1
 </t>
@@ -10549,6 +10919,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 476 MDM 6 TIM 3-1</t>
     </r>
@@ -10661,6 +11032,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DG1(V26-BL10-1,2,3A,4A/V01-7,8,9)DG2(V35-7,8,9/V23-BL01-NV11)CIND_C107_E/3=AE05_C101</t>
     </r>
@@ -10670,6 +11042,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">_E/2</t>
     </r>
@@ -10678,6 +11051,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(V07-H44-4,5,6)</t>
     </r>
@@ -10706,6 +11080,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DG1(V30-BL57-1,2,3A,4B/V01-13,14,15)DG2(V35-13,14,15/V24-BL02-NV12)CIND_C101_</t>
     </r>
@@ -10715,6 +11090,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">C/4</t>
     </r>
@@ -10723,6 +11099,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">=AE05_C101_</t>
     </r>
@@ -10732,6 +11109,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">C/1</t>
     </r>
@@ -10740,6 +11118,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(V07-H41-4,5,6)</t>
     </r>
@@ -10802,6 +11181,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DG1(V31-BL08-1,2,3A,4B/V01-43,44,45)DG2(V35-43,44,45/V23-BL02-NV20)CIND_C109_</t>
     </r>
@@ -10811,6 +11191,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">C/4</t>
     </r>
@@ -10819,6 +11200,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">=AE05_C101_D/3(V07-H43-4,5,6)</t>
     </r>
@@ -10832,6 +11214,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 520 MDM 5 TIM 4-2
 </t>
@@ -10842,6 +11225,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 476 MDM 8 TIM 5-2</t>
     </r>
@@ -10888,6 +11272,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 511 MDM 8 TIM 3-1
 </t>
@@ -10898,6 +11283,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 697 MDM 3 TIM 3-1</t>
     </r>
@@ -10914,6 +11300,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 511 MDM 8 TIM 4-1
 </t>
@@ -10924,6 +11311,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 697 MDM 3 TIM 3-2</t>
     </r>
@@ -10949,6 +11337,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 511 MDM 8 TIM 2-2
 </t>
@@ -10959,6 +11348,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 697 MDM 3 TIM 2-2</t>
     </r>
@@ -10969,6 +11359,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DG1(V25-BL45-6,7,8A,9A/V02-238,239,240)DG2(V02-238,239,240/V16-BL07-NV04</t>
     </r>
@@ -10978,6 +11369,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-PTT está no 4A e o SQ, no 4B do NV04</t>
     </r>
@@ -10986,6 +11378,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -11080,6 +11473,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">120.95 MHz (SFS&lt;&lt;&gt;&gt;DTCEA-CT) </t>
     </r>
@@ -11090,6 +11484,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Não passa pelo C2</t>
     </r>
@@ -11105,6 +11500,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DG da OI no DTCEA-CT&gt;&gt;</t>
     </r>
@@ -11113,6 +11509,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(V15-BL3-N12)AER4_C101_D/4=MDCI_C100_G/1(PP.01-PT.09)</t>
     </r>
@@ -11123,6 +11520,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">&gt;&gt;Patch Panel em São Francisco do Do Sul</t>
     </r>
@@ -11133,6 +11531,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">133.15 MHz (SFS&lt;&lt;&gt;&gt;DTCEA-CT) </t>
     </r>
@@ -11143,6 +11542,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Não passa pelo C2</t>
     </r>
@@ -11158,6 +11558,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DG da OI no DTCEA-CT&gt;&gt;</t>
     </r>
@@ -11166,6 +11567,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(V15-BL3-N18)AER4_C101_F/2=MDCI_C100_G/2(PP.01-PT.10)</t>
     </r>
@@ -11176,6 +11578,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">&gt;&gt;Patch Panel em São Francisco do Do Sul</t>
     </r>
@@ -11308,6 +11711,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 502 MDM 3 TIM 3-1
 </t>
@@ -11318,6 +11722,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 700 MDM 4 TIM 3-1</t>
     </r>
@@ -11356,6 +11761,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 502 MDM 4 TIM 3-2
 </t>
@@ -11366,6 +11772,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 700 MDM 5 TIM 3-2</t>
     </r>
@@ -11446,6 +11853,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">MPLS </t>
     </r>
@@ -11455,6 +11863,7 @@
         <color rgb="FFFFFF66"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(responsável pelo CKT é a MB)</t>
     </r>
@@ -11489,6 +11898,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 502 MDM 2 TIM 2-3
 </t>
@@ -11499,6 +11909,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 482 MDM 2 TIM 1-3</t>
     </r>
@@ -11576,6 +11987,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">D19 </t>
     </r>
@@ -11585,6 +11997,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(Esta freq. existiu por ocasião da Copa do Mundo e das Olimpíadas. Atualmente, não existe na NOSDA do COPM. Segundo Ten. Gustavo, esta freq. será oficializada futuramente com o mesmo desiguinativo)</t>
     </r>
@@ -11625,6 +12038,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 203 MDM 2 TIM 2-3
 </t>
@@ -11635,6 +12049,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 488 MDM 2 TIM 2-3</t>
     </r>
@@ -11648,6 +12063,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">124.275 MHz </t>
     </r>
@@ -11657,6 +12073,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(antes era 121.500 MHz)</t>
     </r>
@@ -11667,6 +12084,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 203 MDM 2 TIM 2-1
 </t>
@@ -11677,6 +12095,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 488 MDM 2 TIM 2-1</t>
     </r>
@@ -11693,6 +12112,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 203 MDM 2 TIM 1-1
 </t>
@@ -11703,6 +12123,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 488 MDM 2 TIM 1-1</t>
     </r>
@@ -11776,6 +12197,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">129.25 MHz </t>
     </r>
@@ -11785,6 +12207,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(Não é mais usada, ckt OI pode ser reaproveitado) </t>
     </r>
@@ -11819,6 +12242,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">123.70 MHz </t>
     </r>
@@ -11828,6 +12252,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> (Não é mais usada, ckt OI pode ser reaproveitado)</t>
     </r>
@@ -12024,6 +12449,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 513 MDM 5 TIM 3-3
 </t>
@@ -12034,6 +12460,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 494 MDM 7 TIM 6-3</t>
     </r>
@@ -12184,6 +12611,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 514 MDM 5 TIM 5-1
 </t>
@@ -12194,6 +12622,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 494 MDM 3 TIM 2-2</t>
     </r>
@@ -12228,6 +12657,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 514 MDM 7 TIM 7-1
 </t>
@@ -12238,6 +12668,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 494 MDM 8 TIM 3-1</t>
     </r>
@@ -12246,6 +12677,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -12265,6 +12697,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 514 MDM 5 TIM 5-2
 </t>
@@ -12275,6 +12708,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 494 MDM 3 TIM 2-1</t>
     </r>
@@ -12291,6 +12725,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CTT 514 MDM 7 TIM 11-1
 </t>
@@ -12301,6 +12736,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RTT 494 MDM 8 TIM 4-1</t>
     </r>
@@ -12317,6 +12753,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">124.775 MHz </t>
     </r>
@@ -12326,6 +12763,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(a conexão entre a SITTI e a OI ainda não foi feita)</t>
     </r>
@@ -12336,6 +12774,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">TCS</t>
     </r>
@@ -12345,6 +12784,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">????????</t>
     </r>
@@ -12424,6 +12864,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">XXX </t>
     </r>
@@ -12433,6 +12874,7 @@
         <color rgb="FFFFFF00"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(Agdo desativação por parte da TEL)</t>
     </r>
@@ -12503,6 +12945,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">APP-VT </t>
     </r>
@@ -12512,6 +12955,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(CONTRATO DE RESPONSABILIDADE DA INFRAERO)</t>
     </r>
@@ -12522,6 +12966,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">DG2(V31-BL55-P09/V35-P360) DG1(V1-P360/V20-BL06-P01)CIIF_C100 SLOT </t>
     </r>
@@ -12531,6 +12976,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">???</t>
     </r>
@@ -12539,6 +12985,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> PORTA </t>
     </r>
@@ -12548,6 +12995,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">???</t>
     </r>
@@ -12556,6 +13004,7 @@
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">=VTA_INFR01-AE01 SLOT ??? PORTA ???</t>
     </r>
@@ -12637,6 +13086,7 @@
       <sz val="8"/>
       <name val="Comic Sans MS"/>
       <family val="4"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -12644,11 +13094,13 @@
       <color rgb="FFEEEEEE"/>
       <name val="Comic Sans MS"/>
       <family val="4"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Comic Sans MS"/>
       <family val="4"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -12656,17 +13108,20 @@
       <color rgb="FFEEEEEE"/>
       <name val="Comic Sans MS"/>
       <family val="4"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -12674,12 +13129,14 @@
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <strike val="true"/>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -12687,12 +13144,14 @@
       <color rgb="FFFF6600"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -12700,52 +13159,61 @@
       <color rgb="FF009933"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="6"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="6"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FFFFFFCC"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FFFFFF00"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FFFF3333"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="7"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FFFF6600"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -12753,12 +13221,14 @@
       <color rgb="FFFFFF00"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <strike val="true"/>
@@ -12766,6 +13236,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -12773,12 +13244,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FFFFFF66"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -12787,6 +13260,7 @@
       <color rgb="FFFFFF99"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -12794,6 +13268,7 @@
       <color rgb="FFFFFF99"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -12801,6 +13276,7 @@
       <color rgb="FFFFFF00"/>
       <name val="Comic Sans MS"/>
       <family val="4"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -12808,6 +13284,7 @@
       <color rgb="FF990000"/>
       <name val="Comic Sans MS"/>
       <family val="4"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -12816,11 +13293,13 @@
       <color rgb="FF990000"/>
       <name val="Comic Sans MS"/>
       <family val="4"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="5"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -12828,6 +13307,7 @@
       <color rgb="FFFF3333"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -12835,6 +13315,7 @@
       <color rgb="FFFFFF00"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -12842,11 +13323,13 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="19">
@@ -13720,11 +14203,11 @@
   </sheetPr>
   <dimension ref="A1:J127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A110" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A128" activeCellId="0" sqref="A128"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.8"/>
@@ -13934,7 +14417,7 @@
         <v>123.725</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>24</v>
@@ -13966,7 +14449,7 @@
         <v>123.725</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
@@ -17813,19 +18296,19 @@
   </sheetPr>
   <dimension ref="A1:H817"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="54.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="109.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>